<commit_message>
Editing the Docs Minor changes in Main_ID
</commit_message>
<xml_diff>
--- a/Utilities/TO DO.xlsx
+++ b/Utilities/TO DO.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darta\Desktop\Bens\Work\Python\JUNC\JUNC#2\FullJUNC\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darta\Desktop\Bens\Work\Python\JUNC\git\JUNC\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58DDB6B7-57D0-4191-93AA-89CE0BFCE9CF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C065DAA8-7484-4657-9B8A-19812C52D682}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{88697885-0CF2-4F57-A352-6C9D3D952390}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="33" uniqueCount="18">
   <si>
     <t>Building_Diagram</t>
   </si>
@@ -132,13 +132,6 @@
   </cellStyles>
   <dxfs count="4">
     <dxf>
-      <font>
-        <b val="0"/>
-        <i val="0"/>
-        <strike/>
-      </font>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill>
           <bgColor theme="9" tint="0.79998168889431442"/>
@@ -158,6 +151,13 @@
           <bgColor theme="7"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+        <strike/>
+      </font>
     </dxf>
   </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -404,158 +404,203 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{661E068B-927F-4214-BFF7-29660A0C6CEE}">
-  <dimension ref="A1:C14"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="15" customWidth="1"/>
-    <col min="2" max="2" width="15.21875" customWidth="1"/>
+    <col min="2" max="2" width="15" customWidth="1"/>
+    <col min="3" max="3" width="15.21875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>16</v>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A1">
+        <v>2</v>
       </c>
       <c r="B1" t="s">
+        <v>16</v>
+      </c>
+      <c r="C1" t="s">
         <v>3</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>16</v>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>4</v>
       </c>
       <c r="B2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
         <v>15</v>
       </c>
-      <c r="B3" t="s">
+      <c r="C3" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>16</v>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
       </c>
       <c r="B4" t="s">
+        <v>16</v>
+      </c>
+      <c r="C4" t="s">
         <v>12</v>
       </c>
-      <c r="C4" t="s">
+      <c r="D4" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>5</v>
+      </c>
+      <c r="B5" t="s">
+        <v>16</v>
+      </c>
+      <c r="C5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D5" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>12</v>
+      </c>
+      <c r="B6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="C6" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>13</v>
+      </c>
+      <c r="B7" t="s">
         <v>14</v>
       </c>
-      <c r="B6" t="s">
+      <c r="C7" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A8">
         <v>14</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B8" t="s">
+        <v>14</v>
+      </c>
+      <c r="C8" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>16</v>
-      </c>
-      <c r="B8" t="s">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>16</v>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>6</v>
       </c>
       <c r="B9" t="s">
+        <v>16</v>
+      </c>
+      <c r="C9" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A10">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
         <v>15</v>
       </c>
-      <c r="B10" t="s">
+      <c r="C10" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A11">
+        <v>8</v>
+      </c>
+      <c r="B11" t="s">
         <v>15</v>
       </c>
-      <c r="B11" t="s">
+      <c r="C11" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>15</v>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A12">
+        <v>7</v>
       </c>
       <c r="B12" t="s">
+        <v>16</v>
+      </c>
+      <c r="C12" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>16</v>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A13">
+        <v>10</v>
       </c>
       <c r="B13" t="s">
+        <v>16</v>
+      </c>
+      <c r="C13" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>16</v>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="A14">
+        <v>9</v>
       </c>
       <c r="B14" t="s">
+        <v>16</v>
+      </c>
+      <c r="C14" t="s">
         <v>13</v>
       </c>
     </row>
   </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:C14">
-    <sortCondition ref="C1:C14"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="B1:D14">
+    <sortCondition ref="D1:D14"/>
   </sortState>
-  <conditionalFormatting sqref="B1:B14">
-    <cfRule type="expression" dxfId="3" priority="2" stopIfTrue="1">
-      <formula>A1="Building"</formula>
+  <conditionalFormatting sqref="C1:C14">
+    <cfRule type="expression" dxfId="3" priority="1" stopIfTrue="1">
+      <formula>D1="V"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="2" priority="3" stopIfTrue="1">
-      <formula>A1="Main"</formula>
+    <cfRule type="expression" dxfId="2" priority="2" stopIfTrue="1">
+      <formula>B1="Building"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="1" priority="4" stopIfTrue="1">
-      <formula>A1="Subclass"</formula>
+    <cfRule type="expression" dxfId="1" priority="3" stopIfTrue="1">
+      <formula>B1="Main"</formula>
     </cfRule>
-    <cfRule type="expression" dxfId="0" priority="1" stopIfTrue="1">
-      <formula>C1="V"</formula>
+    <cfRule type="expression" dxfId="0" priority="4" stopIfTrue="1">
+      <formula>B1="Subclass"</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Editing the Docs for Main table
</commit_message>
<xml_diff>
--- a/Utilities/TO DO.xlsx
+++ b/Utilities/TO DO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darta\Desktop\Bens\Work\Python\JUNC\git\JUNC\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC38965B-4CB0-46AC-976D-7EB6ADD00C17}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{24AAE1F5-2643-4D16-BF8C-2E3429DE2251}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{88697885-0CF2-4F57-A352-6C9D3D952390}"/>
+    <workbookView xWindow="3000" yWindow="720" windowWidth="21600" windowHeight="11340" xr2:uid="{88697885-0CF2-4F57-A352-6C9D3D952390}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -407,7 +407,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+      <selection activeCell="D18" sqref="D18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
Minor edits - fixing different functions with the same name in different files.
</commit_message>
<xml_diff>
--- a/Utilities/TO DO.xlsx
+++ b/Utilities/TO DO.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\darta\Desktop\Bens\Work\Python\JUNC\git\JUNC\Utilities\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{09D1570F-DD2D-41AA-ACF2-26CEBDB32F66}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4875EF2F-9356-4C03-B72A-6E7ED1DCBD18}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12720" xr2:uid="{88697885-0CF2-4F57-A352-6C9D3D952390}"/>
+    <workbookView xWindow="2316" yWindow="2244" windowWidth="17280" windowHeight="9072" xr2:uid="{88697885-0CF2-4F57-A352-6C9D3D952390}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="18">
   <si>
     <t>Building_Diagram</t>
   </si>
@@ -407,7 +407,7 @@
   <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G17" sqref="G17"/>
+      <selection activeCell="F10" sqref="F10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -523,6 +523,9 @@
       </c>
       <c r="C8" t="s">
         <v>0</v>
+      </c>
+      <c r="D8" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.3">

</xml_diff>